<commit_message>
membuat file formulir perubahan untuk standar 6
</commit_message>
<xml_diff>
--- a/uploads/pdf/gangguan/form_gangguan.xlsx
+++ b/uploads/pdf/gangguan/form_gangguan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\standarlpse_17\assets\file\pdf\gangguan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\standarlpse_17\uploads\pdf\gangguan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A2000A5-C322-47D5-81F5-9C00BF83D1F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763A2F40-E099-4920-AB6D-0CC426DB3259}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D7576A1F-7869-4098-980D-EB74C8A93634}"/>
   </bookViews>
@@ -257,14 +257,14 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">                                 FORMULIR PENCATATAN GANGGUAN / MASALAH DAN PERMINTAAN LAYANAN</t>
+    <t xml:space="preserve">                        FORMULIR PENCATATAN GANGGUAN / MASALAH DAN PERMINTAAN LAYANAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,14 +285,6 @@
       <i/>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -465,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -476,14 +468,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -491,176 +570,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1083,15 +1066,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E63A57B-2C7B-46C8-B9FE-25FD0B375F93}">
   <dimension ref="B1:J55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:K55"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="2.7109375" style="1" customWidth="1"/>
@@ -1104,740 +1087,803 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="65"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42" t="s">
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="47"/>
     </row>
     <row r="4" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="45" t="s">
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="50"/>
     </row>
     <row r="5" spans="2:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="31"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="53"/>
     </row>
     <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="35"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="35"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="35"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="27"/>
     </row>
     <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="16"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="28"/>
     </row>
     <row r="12" spans="2:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
     </row>
     <row r="14" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="27"/>
     </row>
     <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="21" t="s">
+      <c r="I15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="23"/>
+      <c r="J15" s="26"/>
     </row>
     <row r="16" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="26"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="59"/>
     </row>
     <row r="17" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="27"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="4"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="2"/>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="26"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
     </row>
     <row r="20" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="C21" s="4"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="21" t="s">
+      <c r="I21" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="J21" s="23"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="19"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="6"/>
     </row>
     <row r="23" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="18"/>
-      <c r="C23" s="4"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F23" s="2"/>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="26"/>
     </row>
     <row r="24" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="18"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="17"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="62"/>
     </row>
     <row r="25" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="6"/>
     </row>
     <row r="26" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="16"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="28"/>
     </row>
     <row r="27" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="10"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="27"/>
     </row>
     <row r="28" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-      <c r="C28" s="4"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="21" t="s">
+      <c r="I28" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="23"/>
+      <c r="J28" s="26"/>
     </row>
     <row r="29" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="28"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="57"/>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="18"/>
-      <c r="C30" s="4"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="19"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="6"/>
     </row>
     <row r="31" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="20"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="26"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="59"/>
     </row>
     <row r="32" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="10"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="27"/>
     </row>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F33" s="2"/>
-      <c r="G33" s="21" t="s">
+      <c r="G33" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="23"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="26"/>
     </row>
     <row r="34" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="14"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="16"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="28"/>
     </row>
     <row r="35" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="10"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="27"/>
     </row>
     <row r="36" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
-      <c r="C36" s="4"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F36" s="2"/>
-      <c r="G36" s="13" t="s">
+      <c r="G36" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H36" s="2"/>
-      <c r="I36" s="21" t="s">
+      <c r="I36" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="J36" s="23"/>
+      <c r="J36" s="26"/>
     </row>
     <row r="37" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="14"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="16"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="28"/>
     </row>
     <row r="38" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="10"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="27"/>
     </row>
     <row r="39" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="11"/>
-      <c r="C39" s="4"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="13" t="s">
+      <c r="E39" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F39" s="2"/>
-      <c r="G39" s="13" t="s">
+      <c r="G39" s="5" t="s">
         <v>33</v>
       </c>
       <c r="H39" s="2"/>
-      <c r="I39" s="21" t="s">
+      <c r="I39" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="J39" s="23"/>
+      <c r="J39" s="26"/>
     </row>
     <row r="40" spans="2:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="14"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="16"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="28"/>
     </row>
     <row r="41" spans="2:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="38"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="31"/>
     </row>
     <row r="43" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="49" t="s">
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="I43" s="50"/>
-      <c r="J43" s="51"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="48" t="s">
+      <c r="B44" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="7" t="s">
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="I44" s="8"/>
-      <c r="J44" s="27"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="38"/>
     </row>
     <row r="45" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="54"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="57"/>
-      <c r="J45" s="58"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="2:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
     </row>
     <row r="47" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="38"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="48" t="s">
+      <c r="B48" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C48" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="7" t="s">
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="I48" s="8"/>
-      <c r="J48" s="27"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="38"/>
     </row>
     <row r="49" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="54"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="57"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="57"/>
-      <c r="J49" s="58"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="35"/>
     </row>
     <row r="50" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="59" t="s">
+      <c r="B50" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="10"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="27"/>
     </row>
     <row r="51" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="21"/>
-      <c r="C51" s="4"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="24"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="13" t="s">
+      <c r="E51" s="5" t="s">
         <v>47</v>
       </c>
       <c r="F51" s="2"/>
-      <c r="G51" s="21" t="s">
+      <c r="G51" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="23"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="26"/>
     </row>
     <row r="52" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="60"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="16"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="28"/>
     </row>
     <row r="53" spans="2:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="9"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
     </row>
     <row r="54" spans="2:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="61" t="s">
+      <c r="B54" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="62" t="s">
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G54" s="34"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="35"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="18"/>
     </row>
     <row r="55" spans="2:10" ht="0.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="9"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="79">
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D22:I22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="D24:J24"/>
+    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:J38"/>
+    <mergeCell ref="D40:J40"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="D37:J37"/>
+    <mergeCell ref="D27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="D32:J32"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="D34:J34"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="D10:J11"/>
+    <mergeCell ref="B42:J42"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
     <mergeCell ref="B55:J55"/>
     <mergeCell ref="B53:J53"/>
     <mergeCell ref="B54:E54"/>
@@ -1854,69 +1900,6 @@
     <mergeCell ref="H44:J44"/>
     <mergeCell ref="H45:J45"/>
     <mergeCell ref="D48:G49"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="D10:J11"/>
-    <mergeCell ref="B42:J42"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:J35"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="D37:J37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:J38"/>
-    <mergeCell ref="D40:J40"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="D27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="D32:J32"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="D34:J34"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D22:I22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="D24:J24"/>
-    <mergeCell ref="D26:J26"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="168" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>

</xml_diff>